<commit_message>
changes for latest grading assistant program, format of rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab02/Lab2Rubric-CS195.xlsx
+++ b/Labs/Lab02/Lab2Rubric-CS195.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CIS195-CourseMaterials\Labs\Lab02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD0EB82E-FAF0-A142-9FEA-71A42C8AD0A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD5C3AD-B025-43E2-B083-04DB49B32783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8440" yWindow="620" windowWidth="15960" windowHeight="15580" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="8400" yWindow="732" windowWidth="14088" windowHeight="15648" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Elements used:</t>
   </si>
@@ -101,6 +112,24 @@
   </si>
   <si>
     <t>Best Practices</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Part 1: One of the review pages</t>
+  </si>
+  <si>
+    <t>Part 2:  The full review site</t>
+  </si>
+  <si>
+    <t>Excellent work!</t>
+  </si>
+  <si>
+    <t>Here's the grade breakdown:</t>
+  </si>
+  <si>
+    <t>Lab 2: A Review web site</t>
   </si>
 </sst>
 </file>
@@ -160,14 +189,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -485,22 +525,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:B24"/>
+    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" customWidth="1"/>
+    <col min="1" max="1" width="19.19921875" customWidth="1"/>
+    <col min="2" max="2" width="7.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -509,71 +549,71 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -582,12 +622,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -595,63 +635,63 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -661,12 +701,12 @@
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -682,257 +722,297 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="18.69921875" customWidth="1"/>
+    <col min="2" max="2" width="6.69921875" customWidth="1"/>
+    <col min="3" max="3" width="7.69921875" customWidth="1"/>
+    <col min="4" max="4" width="1" customWidth="1"/>
+    <col min="5" max="5" width="20.796875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C7">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C8">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C10">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C11">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4">
-        <v>2</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="4">
-        <v>2</v>
-      </c>
-      <c r="C10" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="3">
-        <f>SUM(B3:B10)</f>
+      <c r="B14" s="3">
+        <f>SUM(B6:B13)</f>
         <v>16</v>
       </c>
-      <c r="C11" s="3">
-        <f>SUM(C3:C10)</f>
+      <c r="C14" s="3">
+        <f>SUM(C6:C13)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B18">
         <v>4</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C18">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B19">
         <v>6</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C19">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B20">
         <v>4</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C20">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4">
-        <v>2</v>
-      </c>
-      <c r="C18" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B22">
         <v>4</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C22">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4">
-        <v>2</v>
-      </c>
-      <c r="C20" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="4">
-        <v>2</v>
-      </c>
-      <c r="C21" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
-        <f>SUM(B14:B21)</f>
+      <c r="B25" s="3">
+        <f>SUM(B17:B24)</f>
         <v>24</v>
       </c>
-      <c r="C22" s="3">
-        <f>SUM(C14:C21)</f>
+      <c r="C25" s="3">
+        <f>SUM(C17:C24)</f>
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="1">
-        <f>B11+B22</f>
+      <c r="B26" s="1">
+        <f>B14+B25</f>
         <v>40</v>
       </c>
-      <c r="C23" s="1">
-        <f>C11+C22</f>
+      <c r="C26" s="1">
+        <f>C14+C25</f>
         <v>40</v>
       </c>
+      <c r="D26" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a reset macro to the rubric
</commit_message>
<xml_diff>
--- a/Labs/Lab02/Lab2Rubric-CS195.xlsx
+++ b/Labs/Lab02/Lab2Rubric-CS195.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CIS195-CourseMaterials\Labs\Lab02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD5C3AD-B025-43E2-B083-04DB49B32783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DF9E88-D6A8-48B1-A2B9-96F03D0A25DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="732" windowWidth="14088" windowHeight="15648" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -123,13 +123,13 @@
     <t>Part 2:  The full review site</t>
   </si>
   <si>
+    <t>Here's the grade breakdown:</t>
+  </si>
+  <si>
+    <t>Lab 2: A Review web site</t>
+  </si>
+  <si>
     <t>Excellent work!</t>
-  </si>
-  <si>
-    <t>Here's the grade breakdown:</t>
-  </si>
-  <si>
-    <t>Lab 2: A Review web site</t>
   </si>
 </sst>
 </file>
@@ -200,14 +200,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,9 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -722,44 +723,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.69921875" customWidth="1"/>
-    <col min="2" max="2" width="6.69921875" customWidth="1"/>
+    <col min="2" max="2" width="7.796875" customWidth="1"/>
     <col min="3" max="3" width="7.69921875" customWidth="1"/>
-    <col min="4" max="4" width="1" customWidth="1"/>
+    <col min="4" max="4" width="0.69921875" customWidth="1"/>
     <col min="5" max="5" width="20.796875" style="4" customWidth="1"/>
     <col min="6" max="6" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -771,10 +773,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="5" t="s">
@@ -893,10 +895,10 @@
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5" t="s">

</xml_diff>